<commit_message>
Add a Better Example Data
</commit_message>
<xml_diff>
--- a/Data/all.xlsx
+++ b/Data/all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\e7\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJ\e7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B28DF4-1170-4A2A-ABF3-AF89B65D93E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC533ED-E134-4214-9269-F10BEC671BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="13740" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="13" r:id="rId1"/>
@@ -727,7 +727,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,6 +737,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,7 +803,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -809,12 +833,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -822,6 +840,31 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,13 +1181,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D0734F-A54F-44EC-A207-49C8E4056ABE}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="8" bestFit="1" customWidth="1"/>
@@ -1181,7 +1224,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="7">
@@ -1210,7 +1253,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="7">
@@ -1239,7 +1282,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>91</v>
       </c>
       <c r="B4" s="7">
@@ -1268,7 +1311,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="7">
@@ -1297,7 +1340,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>92</v>
       </c>
       <c r="B6" s="7">
@@ -1326,7 +1369,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>93</v>
       </c>
       <c r="B7" s="7">
@@ -1355,7 +1398,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>73</v>
       </c>
       <c r="B8" s="7">
@@ -1384,7 +1427,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="7">
@@ -1413,7 +1456,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="7">
@@ -1442,7 +1485,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="7">
@@ -1471,7 +1514,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>96</v>
       </c>
       <c r="B12" s="7">
@@ -1500,7 +1543,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>97</v>
       </c>
       <c r="B13" s="7">
@@ -1529,7 +1572,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>98</v>
       </c>
       <c r="B14" s="7">
@@ -1558,7 +1601,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="7">
@@ -1587,7 +1630,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="7">
@@ -1616,7 +1659,7 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B17" s="7">
@@ -1645,7 +1688,7 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="7">
@@ -1674,7 +1717,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="7">
@@ -1703,7 +1746,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B20" s="7">
@@ -1732,7 +1775,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="16" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="7">
@@ -1761,7 +1804,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B22" s="7">
@@ -1790,7 +1833,7 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B23" s="7">
@@ -1819,7 +1862,7 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B24" s="7">
@@ -1848,7 +1891,7 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B25" s="7">
@@ -1877,7 +1920,7 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="17" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="7">
@@ -1906,7 +1949,7 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="16" t="s">
         <v>108</v>
       </c>
       <c r="B27" s="7">
@@ -1935,7 +1978,7 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B28" s="7">
@@ -1964,7 +2007,7 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="7">
@@ -1993,7 +2036,7 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B30" s="7">
@@ -2022,7 +2065,7 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="7">
@@ -2051,7 +2094,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="15" t="s">
         <v>100</v>
       </c>
       <c r="B32" s="7">
@@ -2080,7 +2123,7 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B33" s="7">
@@ -2109,7 +2152,7 @@
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B34" s="7">
@@ -2138,7 +2181,7 @@
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B35" s="7">
@@ -2167,7 +2210,7 @@
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="7">
@@ -2196,7 +2239,7 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B37" s="7">
@@ -2225,7 +2268,7 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B38" s="7">
@@ -2254,7 +2297,7 @@
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B39" s="7">
@@ -2283,7 +2326,7 @@
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B40" s="7">
@@ -2312,7 +2355,7 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B41" s="7">
@@ -2341,7 +2384,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B42" s="7">
@@ -2370,7 +2413,7 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="18" t="s">
         <v>104</v>
       </c>
       <c r="B43" s="7">
@@ -2399,7 +2442,7 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B44" s="7">
@@ -2428,7 +2471,7 @@
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B45" s="7">
@@ -2457,7 +2500,7 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="18" t="s">
         <v>112</v>
       </c>
       <c r="B46" s="7">
@@ -2486,7 +2529,7 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="18" t="s">
         <v>113</v>
       </c>
       <c r="B47" s="7">
@@ -2515,7 +2558,7 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="20" t="s">
         <v>102</v>
       </c>
       <c r="B48" s="7">
@@ -2544,7 +2587,7 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="21" t="s">
         <v>85</v>
       </c>
       <c r="B49" s="7">
@@ -2573,7 +2616,7 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="20" t="s">
         <v>84</v>
       </c>
       <c r="B50" s="7">
@@ -2602,7 +2645,7 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="20" t="s">
         <v>114</v>
       </c>
       <c r="B51" s="7">
@@ -2631,7 +2674,7 @@
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="20" t="s">
         <v>115</v>
       </c>
       <c r="B52" s="7">
@@ -2660,7 +2703,7 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="20" t="s">
         <v>116</v>
       </c>
       <c r="B53" s="7">
@@ -2689,7 +2732,7 @@
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B54" s="7">
@@ -2718,7 +2761,7 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="20" t="s">
         <v>89</v>
       </c>
       <c r="B55" s="7">
@@ -2747,7 +2790,7 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="20" t="s">
         <v>118</v>
       </c>
       <c r="B56" s="7">
@@ -2776,7 +2819,7 @@
       </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B57" s="7">
@@ -2805,7 +2848,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" s="2" customFormat="1">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="18" t="s">
         <v>120</v>
       </c>
       <c r="B58" s="7">
@@ -2834,7 +2877,7 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="22" t="s">
         <v>121</v>
       </c>
       <c r="B59" s="8">
@@ -2863,7 +2906,7 @@
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="20" t="s">
         <v>103</v>
       </c>
       <c r="B60" s="7">
@@ -16514,7 +16557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC8F736-B5AD-48FD-B4FA-92857C55BAC7}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>

</xml_diff>